<commit_message>
updated first two scenarios
</commit_message>
<xml_diff>
--- a/src/test.demoApi/resources/testData/demoData.xlsx
+++ b/src/test.demoApi/resources/testData/demoData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aturuk\IdeaProjects\mtf-automation-testing-api\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mthomas\Documents\mtf-dm-automation-test-api\src\test.demoApi\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8831416E-2501-4279-88D8-394C2838D112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6D0137-82C6-47A8-BC54-27DD9DC6E67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3FAEF57A-74CB-4873-83C5-7175CED35448}"/>
+    <workbookView xWindow="3036" yWindow="2664" windowWidth="17280" windowHeight="8880" xr2:uid="{3FAEF57A-74CB-4873-83C5-7175CED35448}"/>
   </bookViews>
   <sheets>
     <sheet name="Create" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>SU-TC001</t>
   </si>
@@ -201,6 +201,18 @@
   </si>
   <si>
     <t>SECOND</t>
+  </si>
+  <si>
+    <t>STATUS_CODE</t>
+  </si>
+  <si>
+    <t>createdAt</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>2024</t>
   </si>
 </sst>
 </file>
@@ -252,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -261,6 +273,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E585723F-DA52-4C5A-A7AB-E6B3EDE8D02A}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -586,9 +599,11 @@
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.77734375" customWidth="1"/>
     <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -598,8 +613,14 @@
       <c r="C1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -609,8 +630,14 @@
       <c r="C2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -620,8 +647,14 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -631,8 +664,14 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -641,6 +680,12 @@
       </c>
       <c r="C5" t="s">
         <v>26</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -653,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2BE7BE-A976-41FA-902B-902773C98133}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>